<commit_message>
upload 091024 - inflation correciton
</commit_message>
<xml_diff>
--- a/Data Structure.xlsx
+++ b/Data Structure.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pro\Desktop\TSV Data\CSV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pro\Desktop\neueFische - Data Analyst\Capstone\data_analytics_24_4-Capstone_Movie_Group\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CB7DA2-6A99-43E8-8B32-9D65471B34AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B96267D-E91C-4DF3-9105-45C9AB3D835D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-17205" windowWidth="51840" windowHeight="21120" xr2:uid="{57442AFA-0330-478A-B2DC-11E631F1C051}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Main" sheetId="1" r:id="rId1"/>
+    <sheet name="Tables" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="81">
   <si>
     <t>filename</t>
   </si>
@@ -238,6 +239,45 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>IMDB</t>
+  </si>
+  <si>
+    <t>gross</t>
+  </si>
+  <si>
+    <t>release group</t>
+  </si>
+  <si>
+    <t>(Original release, re-relese, country lifetime gross)</t>
+  </si>
+  <si>
+    <t>producing country</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>tickets sold</t>
+  </si>
+  <si>
+    <t>tickets sold since '96</t>
+  </si>
+  <si>
+    <t>BoxOfficeMojo (Top 200 per year)</t>
+  </si>
+  <si>
+    <t>European Data - lumiere (Top 200 per year) EU</t>
+  </si>
+  <si>
+    <t>North American Data - The Numbers (Top 200 per year)  NA</t>
+  </si>
+  <si>
+    <t>release-date</t>
+  </si>
+  <si>
+    <t>gross sales</t>
   </si>
 </sst>
 </file>
@@ -267,7 +307,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -304,8 +344,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -366,57 +430,177 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -732,356 +916,768 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E68F064-934C-498D-A873-951FF8F236F9}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I24" sqref="E24:I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="25" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="11.42578125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+    </row>
+    <row r="3" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M3" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
-        <v>1</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
-        <v>2</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="15"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
+        <v>1</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <v>2</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="18"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B6" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D6" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E6" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G6" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I6" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M6" s="11" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
-        <v>4</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
-        <v>5</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="H6" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="20">
+        <v>5</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B9" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C9" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D9" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E9" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F9" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H9" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I9" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J9" s="11" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B10" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C10" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D10" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E10" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F10" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G10" s="11" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C11" s="3" t="s">
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C13" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E13" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C12" s="2" t="s">
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C14" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D14" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E14" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C13" s="2" t="s">
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C15" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D15" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E15" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E19" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H20" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E24" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="26"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E27" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E28" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>74</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="7">
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A22:M22"/>
+    <mergeCell ref="A26:M26"/>
+    <mergeCell ref="E15:M15"/>
+    <mergeCell ref="E14:M14"/>
     <mergeCell ref="E13:M13"/>
-    <mergeCell ref="E12:M12"/>
-    <mergeCell ref="E11:M11"/>
+    <mergeCell ref="A17:M17"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{845BA6C9-6CC6-4E35-9DD4-3E7A77D1C32E}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" style="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="34"/>
+    <col min="3" max="3" width="9.5703125" style="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="34"/>
+    <col min="5" max="5" width="13.5703125" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="34"/>
+    <col min="7" max="7" width="13.85546875" style="33" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="34"/>
+    <col min="9" max="9" width="17.42578125" style="33" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" style="33" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="11.42578125" style="29"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="30"/>
+      <c r="E1" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="30"/>
+      <c r="G1" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="30"/>
+      <c r="I1" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="29"/>
+      <c r="K1" s="43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="31"/>
+      <c r="E2" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="31"/>
+      <c r="G2" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="31"/>
+      <c r="I2" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="29"/>
+      <c r="K2" s="38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="31"/>
+      <c r="C3" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="31"/>
+      <c r="E3" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="31"/>
+      <c r="G3" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="31"/>
+      <c r="I3" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="29"/>
+      <c r="K3" s="41" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="31"/>
+      <c r="C4" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="31"/>
+      <c r="E4" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="31"/>
+      <c r="G4" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="31"/>
+      <c r="I4" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="29"/>
+      <c r="K4" s="41" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="31"/>
+      <c r="I5" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="29"/>
+      <c r="K5" s="41" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="31"/>
+      <c r="I6" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="29"/>
+      <c r="K6" s="41" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" s="31"/>
+      <c r="I7" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="29"/>
+      <c r="K7" s="41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="41" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="42" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="32"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J11" s="29"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>